<commit_message>
Add a source for the rounding sol'n; re-save test sheets just to be safe
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/datetime-rounding.xlsx
+++ b/tests/testthat/sheets/datetime-rounding.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -392,6 +392,24 @@
         <v>2016-03-23 09:50:00</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>42737.479166666664</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B5" si="0">TEXT(A4,"yyyy-mm-dd hh:mm:ss")</f>
+        <v>2017-01-02 11:30:00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42738.479166666664</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>2017-01-03 11:30:00</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>